<commit_message>
Various updates in the hunt of bugs
</commit_message>
<xml_diff>
--- a/classical_laminate_theory/CLT_input_layup_data/test_layup_1.xlsx
+++ b/classical_laminate_theory/CLT_input_layup_data/test_layup_1.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_composite_toolbox\classical_laminate_theory\CLT_input_layup_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_composite_toolbox\classical_laminate_theory\CLT_input_layup_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C02A00D-A08F-4678-A65B-A1665C7203F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9E0B40-A0A6-4DDF-9996-5C5BB54EA392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="2490" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>layer_no</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>orientation</t>
-  </si>
-  <si>
-    <t>thickness</t>
   </si>
 </sst>
 </file>
@@ -358,12 +355,12 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -373,48 +370,41 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Ey in main_laminate
</commit_message>
<xml_diff>
--- a/classical_laminate_theory/CLT_input_layup_data/test_layup_1.xlsx
+++ b/classical_laminate_theory/CLT_input_layup_data/test_layup_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_composite_toolbox\classical_laminate_theory\CLT_input_layup_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C71D62-1F7D-48CD-8765-16391D70E911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7538B2B-E07F-4583-889C-11C62F534A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -391,17 +391,44 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>